<commit_message>
add top vs weighted sampling hyperparameter
</commit_message>
<xml_diff>
--- a/results/multi_eval_metrics.xlsx
+++ b/results/multi_eval_metrics.xlsx
@@ -492,352 +492,352 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.9629</v>
+        <v>0.9226</v>
       </c>
       <c r="B2" t="n">
-        <v>0.9073</v>
+        <v>0.9772</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7836734693877551</v>
+        <v>0.2214285714285714</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01762749445676275</v>
+        <v>0.001219512195121951</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9823725055432373</v>
+        <v>0.998780487804878</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2163265306122449</v>
+        <v>0.7785714285714286</v>
       </c>
       <c r="G2" t="n">
-        <v>0.75</v>
+        <v>0.01441677588466579</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9823725055432373</v>
+        <v>0.998780487804878</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4006504819222589</v>
+        <v>0.1113240418118467</v>
       </c>
       <c r="J2" t="n">
-        <v>0.97663396891877</v>
+        <v>0.921919770773639</v>
       </c>
       <c r="K2" t="n">
-        <v>0.02336603108123003</v>
+        <v>0.07808022922636104</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.9741</v>
+        <v>0.9360000000000001</v>
       </c>
       <c r="B3" t="n">
-        <v>0.8804</v>
+        <v>0.9429</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9127753303964757</v>
+        <v>0.4696035242290749</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01804850535815003</v>
+        <v>0.004286520022560632</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9819514946418499</v>
+        <v>0.9957134799774394</v>
       </c>
       <c r="F3" t="n">
-        <v>0.08722466960352426</v>
+        <v>0.5303964757709252</v>
       </c>
       <c r="G3" t="n">
-        <v>1.616161616161616</v>
+        <v>0.06312292358803986</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9819514946418499</v>
+        <v>0.9957134799774394</v>
       </c>
       <c r="I3" t="n">
-        <v>0.4654119178773129</v>
+        <v>0.2369450221258178</v>
       </c>
       <c r="J3" t="n">
-        <v>0.9887551113130395</v>
+        <v>0.9361544172234595</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0112448886869605</v>
+        <v>0.06384558277654051</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.9512</v>
+        <v>0.9258</v>
       </c>
       <c r="B4" t="n">
-        <v>0.9299999999999999</v>
+        <v>0.9462</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6027131782945736</v>
+        <v>0.4011627906976744</v>
       </c>
       <c r="D4" t="n">
-        <v>0.008697591436217662</v>
+        <v>0.01382694023193577</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9913024085637824</v>
+        <v>0.9861730597680642</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3972868217054264</v>
+        <v>0.5988372093023255</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1902439024390244</v>
+        <v>0.2006472491909385</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9913024085637824</v>
+        <v>0.9861730597680642</v>
       </c>
       <c r="I4" t="n">
-        <v>0.3057053848653956</v>
+        <v>0.2074948654648051</v>
       </c>
       <c r="J4" t="n">
-        <v>0.9559139784946237</v>
+        <v>0.9346861128725428</v>
       </c>
       <c r="K4" t="n">
-        <v>0.04408602150537633</v>
+        <v>0.06531388712745723</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.9665</v>
+        <v>0.9468</v>
       </c>
       <c r="B5" t="n">
-        <v>0.8799</v>
+        <v>0.9064</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9287128712871288</v>
+        <v>0.7</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02925472747497219</v>
+        <v>0.02547274749721913</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9707452725250278</v>
+        <v>0.9745272525027808</v>
       </c>
       <c r="F5" t="n">
-        <v>0.07128712871287124</v>
+        <v>0.3</v>
       </c>
       <c r="G5" t="n">
-        <v>3.652777777777778</v>
+        <v>0.7557755775577558</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9707452725250278</v>
+        <v>0.9745272525027808</v>
       </c>
       <c r="I5" t="n">
-        <v>0.4789837993810505</v>
+        <v>0.3627363737486096</v>
       </c>
       <c r="J5" t="n">
-        <v>0.99181725196045</v>
+        <v>0.9665710503089144</v>
       </c>
       <c r="K5" t="n">
-        <v>0.008182748039549992</v>
+        <v>0.03342894969108556</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.8556</v>
+        <v>0.9091</v>
       </c>
       <c r="B6" t="n">
-        <v>0.7596000000000001</v>
+        <v>0.9772999999999999</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9887983706720977</v>
+        <v>0.1527494908350306</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1589044133954313</v>
+        <v>0.008538478598358839</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8410955866045686</v>
+        <v>0.9914615214016411</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01120162932790225</v>
+        <v>0.8472505091649695</v>
       </c>
       <c r="G6" t="n">
-        <v>130.2727272727273</v>
+        <v>0.09254807692307693</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8410955866045686</v>
+        <v>0.9914615214016411</v>
       </c>
       <c r="I6" t="n">
-        <v>0.5738513920337646</v>
+        <v>0.08064398471669471</v>
       </c>
       <c r="J6" t="n">
-        <v>0.99855186940495</v>
+        <v>0.9148674920699887</v>
       </c>
       <c r="K6" t="n">
-        <v>0.001448130595050001</v>
+        <v>0.08513250793001126</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.968</v>
+        <v>0.8744</v>
       </c>
       <c r="B7" t="n">
-        <v>0.8898</v>
+        <v>0.8002</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9383408071748879</v>
+        <v>0.9159192825112108</v>
       </c>
       <c r="D7" t="n">
-        <v>0.02909530083443127</v>
+        <v>0.1296662274923145</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9709046991655688</v>
+        <v>0.8703337725076855</v>
       </c>
       <c r="F7" t="n">
-        <v>0.06165919282511212</v>
+        <v>0.0840807174887892</v>
       </c>
       <c r="G7" t="n">
-        <v>4.818181818181818</v>
+        <v>15.74666666666667</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9709046991655688</v>
+        <v>0.8703337725076855</v>
       </c>
       <c r="I7" t="n">
-        <v>0.4837180540046596</v>
+        <v>0.5227927550017626</v>
       </c>
       <c r="J7" t="n">
-        <v>0.9938188356934142</v>
+        <v>0.990627343164209</v>
       </c>
       <c r="K7" t="n">
-        <v>0.006181164306585774</v>
+        <v>0.009372656835791027</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.9559</v>
+        <v>0.9414</v>
       </c>
       <c r="B8" t="n">
-        <v>0.9255</v>
+        <v>0.8673999999999999</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6586638830897703</v>
+        <v>0.8862212943632568</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0126078301260783</v>
+        <v>0.05275381552753815</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9873921698739216</v>
+        <v>0.9472461844724619</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3413361169102297</v>
+        <v>0.1137787056367432</v>
       </c>
       <c r="G8" t="n">
-        <v>0.3486238532110092</v>
+        <v>4.376146788990826</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9873921698739216</v>
+        <v>0.9472461844724619</v>
       </c>
       <c r="I8" t="n">
-        <v>0.3356358566079243</v>
+        <v>0.4694875549453975</v>
       </c>
       <c r="J8" t="n">
-        <v>0.9646677471636953</v>
+        <v>0.9874337099377449</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0353322528363047</v>
+        <v>0.01256629006225507</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.9540999999999999</v>
+        <v>0.8435</v>
       </c>
       <c r="B9" t="n">
-        <v>0.8805000000000001</v>
+        <v>0.7519</v>
       </c>
       <c r="C9" t="n">
-        <v>0.857976653696498</v>
+        <v>0.9455252918287937</v>
       </c>
       <c r="D9" t="n">
-        <v>0.03488631297369595</v>
+        <v>0.1681899242086491</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9651136870263041</v>
+        <v>0.8318100757913509</v>
       </c>
       <c r="F9" t="n">
-        <v>0.142023346303502</v>
+        <v>0.05447470817120625</v>
       </c>
       <c r="G9" t="n">
-        <v>2.143835616438356</v>
+        <v>26.94642857142857</v>
       </c>
       <c r="H9" t="n">
-        <v>0.9651136870263041</v>
+        <v>0.8318100757913509</v>
       </c>
       <c r="I9" t="n">
-        <v>0.446431483335097</v>
+        <v>0.5568576080187214</v>
       </c>
       <c r="J9" t="n">
-        <v>0.9834185122089721</v>
+        <v>0.9925522010905705</v>
       </c>
       <c r="K9" t="n">
-        <v>0.01658148779102786</v>
+        <v>0.007447798909429482</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.9394</v>
+        <v>0.9146</v>
       </c>
       <c r="B10" t="n">
-        <v>0.947</v>
+        <v>0.8902</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4609856262833675</v>
+        <v>0.6252566735112937</v>
       </c>
       <c r="D10" t="n">
-        <v>0.008974074894748505</v>
+        <v>0.05417682251274097</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9910259251052514</v>
+        <v>0.9458231774872591</v>
       </c>
       <c r="F10" t="n">
-        <v>0.5390143737166324</v>
+        <v>0.3747433264887063</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1542857142857143</v>
+        <v>1.33972602739726</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9910259251052514</v>
+        <v>0.9458231774872591</v>
       </c>
       <c r="I10" t="n">
-        <v>0.234979850589058</v>
+        <v>0.3397167480120173</v>
       </c>
       <c r="J10" t="n">
-        <v>0.9445617740232313</v>
+        <v>0.9589979779824759</v>
       </c>
       <c r="K10" t="n">
-        <v>0.05543822597676873</v>
+        <v>0.04100202201752412</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.8991</v>
+        <v>0.8915999999999999</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>0.9403</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.2586719524281467</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>0.0373707040373707</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>0.9626292959626293</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0.7413280475718533</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>0.4491978609625669</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>0.9626292959626293</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>0.1480213282327587</v>
       </c>
       <c r="J11" t="n">
-        <v>0.8991</v>
+        <v>0.9204509199191747</v>
       </c>
       <c r="K11" t="n">
-        <v>0.1009</v>
+        <v>0.07954908008082529</v>
       </c>
     </row>
   </sheetData>

</xml_diff>